<commit_message>
Looping error PO number TSC
</commit_message>
<xml_diff>
--- a/Finished/TSC/Tractor Supply ASN 9016040237 10.22.2024.xlsx
+++ b/Finished/TSC/Tractor Supply ASN 9016040237 10.22.2024.xlsx
@@ -1635,7 +1635,9 @@
           <t>Total Weight</t>
         </is>
       </c>
-      <c r="E13" s="17" t="n"/>
+      <c r="E13" s="17" t="n">
+        <v>1</v>
+      </c>
       <c r="F13" s="15" t="n"/>
       <c r="G13" s="15" t="n"/>
       <c r="H13" s="15" t="n"/>

</xml_diff>